<commit_message>
Solo lee el archivo excel con los registros en el
</commit_message>
<xml_diff>
--- a/depuracion/testdata/testdata.xlsx
+++ b/depuracion/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrosario\git\depuracion\depuracion\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DDE17A-9DB0-4E36-B5BB-692952D202DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63565324-D9BA-42B6-9901-4A653516F16E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5240" xr2:uid="{11FCAED0-D6E0-4838-AFE2-6225B34084DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>usuario</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>jairistasdfsdfdddasddssas@aol.com</t>
+  </si>
+  <si>
+    <t>resultado</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F06A6-C0F3-400D-865C-6573AF119AFD}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +424,7 @@
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -428,21 +434,36 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FC050264-5E28-4AC1-94C7-7437CF42103B}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{FC050264-5E28-4AC1-94C7-7437CF42103B}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{D7BB5D5E-2045-4748-99F6-3C78723DFA3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios para ejecutar desde excel.
</commit_message>
<xml_diff>
--- a/depuracion/testdata/testdata.xlsx
+++ b/depuracion/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrosario\git\depuracion\depuracion\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63565324-D9BA-42B6-9901-4A653516F16E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2E5C7F-01E8-4EDC-8E4A-0C5F4705B4D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5240" xr2:uid="{11FCAED0-D6E0-4838-AFE2-6225B34084DD}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>Login</t>
   </si>
   <si>
-    <t>jairistasdfsdfdddasddssas@aol.com</t>
-  </si>
-  <si>
     <t>resultado</t>
+  </si>
+  <si>
+    <t>jairidssas@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -443,7 +443,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>

</xml_diff>